<commit_message>
modified procedure to activate R environment + working directory changed
</commit_message>
<xml_diff>
--- a/code/tables/descriptives.xlsx
+++ b/code/tables/descriptives.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippe/Desktop/base2/code/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippe/Desktop/projects/base2/code/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAB0E22-3A8E-1B46-90C7-FF99D2EF3CF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911B8799-F928-784C-9B34-01B0924CD0AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="17040" xr2:uid="{51CF6FDD-8525-EE49-8C93-56A1AAE11C86}"/>
   </bookViews>
@@ -2952,31 +2952,31 @@
         <v>332</v>
       </c>
       <c r="D31" s="1">
-        <v>2.5128514056224902</v>
+        <v>2.6451137884872802</v>
       </c>
       <c r="E31" s="1">
-        <v>0.73517145810363205</v>
+        <v>0.69439933930207298</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
       </c>
       <c r="G31" s="1">
-        <v>4.8571428571428603</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="H31" s="1">
-        <v>2</v>
+        <v>2.1749999999999998</v>
       </c>
       <c r="I31" s="1">
-        <v>2.4285714285714302</v>
+        <v>2.65</v>
       </c>
       <c r="J31" s="1">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="K31" s="1">
-        <v>0.435331871927637</v>
+        <v>0.34315607081937599</v>
       </c>
       <c r="L31" s="1">
-        <v>-3.5021909572923199E-2</v>
+        <v>0.13211102018389001</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>58</v>
@@ -3135,11 +3135,11 @@
       </c>
       <c r="Q34" s="3" t="str">
         <f t="shared" ref="Q34:Y35" si="38">SUBSTITUTE(TEXT(D31,"###0.00"),",",".")</f>
-        <v>2.51</v>
+        <v>2.65</v>
       </c>
       <c r="R34" s="3" t="str">
         <f t="shared" si="38"/>
-        <v>0.74</v>
+        <v>0.69</v>
       </c>
       <c r="S34" s="3" t="str">
         <f t="shared" si="38"/>
@@ -3147,27 +3147,27 @@
       </c>
       <c r="T34" s="3" t="str">
         <f t="shared" si="38"/>
-        <v>4.86</v>
+        <v>4.90</v>
       </c>
       <c r="U34" s="3" t="str">
         <f t="shared" si="38"/>
-        <v>2.00</v>
+        <v>2.18</v>
       </c>
       <c r="V34" s="3" t="str">
         <f t="shared" si="38"/>
-        <v>2.43</v>
+        <v>2.65</v>
       </c>
       <c r="W34" s="3" t="str">
         <f t="shared" si="38"/>
-        <v>3.00</v>
+        <v>3.10</v>
       </c>
       <c r="X34" s="3" t="str">
         <f t="shared" si="38"/>
-        <v>0.44</v>
+        <v>0.34</v>
       </c>
       <c r="Y34" s="3" t="str">
         <f t="shared" si="38"/>
-        <v>-0.04</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="35" spans="15:25" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
re-run analyses and added minor code updates
</commit_message>
<xml_diff>
--- a/code/tables/descriptives.xlsx
+++ b/code/tables/descriptives.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippe/Desktop/projects/base2/code/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911B8799-F928-784C-9B34-01B0924CD0AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8394F26-035C-7442-8245-4E7FD6568EB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="17040" xr2:uid="{51CF6FDD-8525-EE49-8C93-56A1AAE11C86}"/>
   </bookViews>
@@ -90,9 +90,6 @@
     <t>Metabolic load factor</t>
   </si>
   <si>
-    <t>Digit symbol task</t>
-  </si>
-  <si>
     <t>Episodic memory</t>
   </si>
   <si>
@@ -264,16 +261,19 @@
     <t>Post-load glucose</t>
   </si>
   <si>
-    <t>Gamma-glutamyltransferase</t>
-  </si>
-  <si>
-    <t>Urea</t>
-  </si>
-  <si>
     <t>controls: 294, cases: 34</t>
   </si>
   <si>
     <t>Tumor necrosis factor-alpha</t>
+  </si>
+  <si>
+    <t>Gamma-glutamyl-transferase</t>
+  </si>
+  <si>
+    <t>Uric acid</t>
+  </si>
+  <si>
+    <t>Digit symbol substitution test</t>
   </si>
 </sst>
 </file>
@@ -661,39 +661,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6EEE9E8-6578-B34F-87B6-283F8C1321ED}">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>4</v>
@@ -705,31 +707,31 @@
         <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>4</v>
@@ -741,18 +743,18 @@
         <v>6</v>
       </c>
       <c r="X2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y2" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1">
         <v>335</v>
@@ -785,7 +787,7 @@
         <v>-0.18902815465998299</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O3" s="5" t="str">
         <f t="shared" ref="O3:P5" si="0">B3</f>
@@ -834,10 +836,10 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="1">
         <v>335</v>
@@ -870,7 +872,7 @@
         <v>-8.2584532221059007E-2</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O4" s="5" t="str">
         <f t="shared" si="0"/>
@@ -919,10 +921,10 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="1">
         <v>335</v>
@@ -955,7 +957,7 @@
         <v>-0.28578817084043201</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O5" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1004,10 +1006,10 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1">
         <v>300</v>
@@ -1040,7 +1042,7 @@
         <v>-1.2940627027060101</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O6" s="5"/>
       <c r="P6" s="3"/>
@@ -1056,10 +1058,10 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1">
         <v>221</v>
@@ -1092,7 +1094,7 @@
         <v>8.3214777042120307</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O7" s="5" t="str">
         <f t="shared" ref="O7:O27" si="18">B6</f>
@@ -1177,7 +1179,7 @@
         <v>11.7532810321888</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O8" s="5" t="str">
         <f t="shared" si="18"/>
@@ -1262,7 +1264,7 @@
         <v>5.1505141874777198</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O9" s="5" t="str">
         <f t="shared" si="18"/>
@@ -1347,7 +1349,7 @@
         <v>2.2894349645404701</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O10" s="5" t="str">
         <f t="shared" si="18"/>
@@ -1396,10 +1398,10 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="1">
         <v>278</v>
@@ -1432,7 +1434,7 @@
         <v>1.6148015624091401</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O11" s="5" t="str">
         <f t="shared" si="18"/>
@@ -1481,7 +1483,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>10</v>
@@ -1517,7 +1519,7 @@
         <v>-1.0952363590409</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O12" s="5" t="str">
         <f t="shared" si="18"/>
@@ -1542,7 +1544,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
@@ -1578,7 +1580,7 @@
         <v>2.3114002315514801</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O13" s="5" t="str">
         <f t="shared" si="18"/>
@@ -1603,7 +1605,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
@@ -1639,7 +1641,7 @@
         <v>6.6804549816366103</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O14" s="5" t="str">
         <f t="shared" si="18"/>
@@ -1664,7 +1666,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
@@ -1700,7 +1702,7 @@
         <v>4.85463049400978</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="O15" s="5" t="str">
         <f t="shared" si="18"/>
@@ -1725,10 +1727,10 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="1">
         <v>318</v>
@@ -1761,7 +1763,7 @@
         <v>104.35702101299</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O16" s="5" t="str">
         <f t="shared" si="18"/>
@@ -1786,10 +1788,10 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1">
         <v>322</v>
@@ -1822,7 +1824,7 @@
         <v>15.7378597719498</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O17" s="5" t="str">
         <f t="shared" si="18"/>
@@ -1871,10 +1873,10 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="1">
         <v>294</v>
@@ -1907,7 +1909,7 @@
         <v>16.933945338913599</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O18" s="5" t="str">
         <f t="shared" si="18"/>
@@ -1956,10 +1958,10 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="1">
         <v>276</v>
@@ -1992,7 +1994,7 @@
         <v>3.47251528376021</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O19" s="5" t="str">
         <f t="shared" si="18"/>
@@ -2041,7 +2043,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
@@ -2077,7 +2079,7 @@
         <v>0.47197729365082602</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O20" s="5" t="str">
         <f t="shared" si="18"/>
@@ -2126,7 +2128,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>14</v>
@@ -2162,7 +2164,7 @@
         <v>1.11463087024064</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O21" s="5" t="str">
         <f t="shared" si="18"/>
@@ -2211,7 +2213,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>15</v>
@@ -2247,7 +2249,7 @@
         <v>0.736875116321698</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O22" s="5" t="str">
         <f t="shared" si="18"/>
@@ -2296,7 +2298,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>17</v>
@@ -2332,7 +2334,7 @@
         <v>6.1407203184323604</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O23" s="5" t="str">
         <f t="shared" si="18"/>
@@ -2381,10 +2383,10 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C24" s="1">
         <v>327</v>
@@ -2417,7 +2419,7 @@
         <v>30.4886928186041</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O24" s="5" t="str">
         <f t="shared" si="18"/>
@@ -2466,10 +2468,10 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C25" s="1">
         <v>327</v>
@@ -2502,11 +2504,11 @@
         <v>0.46076034020606998</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O25" s="5" t="str">
         <f t="shared" si="18"/>
-        <v>Gamma-glutamyltransferase</v>
+        <v>Gamma-glutamyl-transferase</v>
       </c>
       <c r="P25" s="3">
         <f t="shared" si="19"/>
@@ -2551,10 +2553,10 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1">
         <v>307</v>
@@ -2587,11 +2589,11 @@
         <v>124.14578806485</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O26" s="5" t="str">
         <f t="shared" si="18"/>
-        <v>Urea</v>
+        <v>Uric acid</v>
       </c>
       <c r="P26" s="3">
         <f t="shared" si="19"/>
@@ -2636,10 +2638,10 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="C27" s="1">
         <v>324</v>
@@ -2672,7 +2674,7 @@
         <v>1.04400758493934</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O27" s="5" t="str">
         <f t="shared" si="18"/>
@@ -2721,10 +2723,10 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="1">
         <v>335</v>
@@ -2757,7 +2759,7 @@
         <v>-0.130872195875813</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O28" s="5"/>
       <c r="P28" s="3"/>
@@ -2773,10 +2775,10 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" s="1">
         <v>335</v>
@@ -2809,11 +2811,11 @@
         <v>0.11331875106780701</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O29" s="5" t="str">
         <f t="shared" ref="O29:P31" si="32">B27</f>
-        <v>Digit symbol task</v>
+        <v>Digit symbol substitution test</v>
       </c>
       <c r="P29" s="3">
         <f t="shared" si="32"/>
@@ -2858,10 +2860,10 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30" s="1">
         <v>335</v>
@@ -2894,7 +2896,7 @@
         <v>-0.177230048442513</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O30" s="5" t="str">
         <f t="shared" si="32"/>
@@ -2943,10 +2945,10 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="1">
         <v>332</v>
@@ -2979,7 +2981,7 @@
         <v>0.13211102018389001</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O31" s="5" t="str">
         <f t="shared" si="32"/>
@@ -3031,7 +3033,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32" s="1">
         <v>335</v>
@@ -3064,7 +3066,7 @@
         <v>0.18755049512894001</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O32" s="5" t="str">
         <f t="shared" ref="O32:P32" si="36">B30</f>

</xml_diff>